<commit_message>
ch2 topic other essential features and chapter assignments completed
</commit_message>
<xml_diff>
--- a/CodeBasics-Excel-GitHub/PracticeSets/Excel_Basics-1_My_Expense_Budget.xlsx
+++ b/CodeBasics-Excel-GitHub/PracticeSets/Excel_Basics-1_My_Expense_Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shubham-Data-Analytics\Data-Analytics-GitHub\CodeBasics-Excel-GitHub\PracticeSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F15DA67-C398-4DA7-9867-7408FAB9F999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD4C3BD-1D02-4F3E-872C-3D4E5722D4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{4813ED4B-01F4-46B2-90B4-B4775552A3A2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="824" activeTab="7" xr2:uid="{4813ED4B-01F4-46B2-90B4-B4775552A3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="May2024" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Charts 2" sheetId="4" r:id="rId4"/>
     <sheet name="Chart 3" sheetId="5" r:id="rId5"/>
     <sheet name="Chart 4" sheetId="6" r:id="rId6"/>
+    <sheet name="Income Statement" sheetId="7" r:id="rId7"/>
+    <sheet name="Employee Salary" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'May2024'!$A$2:$K$2</definedName>
@@ -34,8 +36,8 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId7"/>
-        <x14:slicerCache r:id="rId8"/>
+        <x14:slicerCache r:id="rId9"/>
+        <x14:slicerCache r:id="rId10"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="50">
   <si>
     <t>Subway Sandwith</t>
   </si>
@@ -164,15 +166,61 @@
   <si>
     <t>NO</t>
   </si>
+  <si>
+    <t xml:space="preserve"> - Cost of Goods Sold (COGS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Selling, general and administrative (SG&amp;A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Depreciation and amortization</t>
+  </si>
+  <si>
+    <t>Operating Income</t>
+  </si>
+  <si>
+    <t>Operating Income %</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Mohan</t>
+  </si>
+  <si>
+    <t>Laila</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Total Compensation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="[$₹-4009]\ #,##0.00"/>
+    <numFmt numFmtId="171" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,8 +236,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,8 +281,20 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -244,11 +311,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -264,52 +347,83 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="15">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -503,111 +617,25 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1229,6 +1257,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0851-484D-B4F4-26F702911D77}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1271,6 +1304,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0851-484D-B4F4-26F702911D77}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1313,6 +1351,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0851-484D-B4F4-26F702911D77}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -6629,8 +6672,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DF222CC3-F2AB-4D26-B7A4-D724D31BF359}" name="MyExpenses" displayName="MyExpenses" ref="A1:E14" totalsRowCount="1">
   <autoFilter ref="A1:E13" xr:uid="{DF222CC3-F2AB-4D26-B7A4-D724D31BF359}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5DA20084-509B-4269-A225-0ED3AF576070}" name="Date" totalsRowLabel="Total" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{1A6423D5-5B54-4F48-8C10-0A81788A91C7}" name="Category" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{5DA20084-509B-4269-A225-0ED3AF576070}" name="Date" totalsRowLabel="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1A6423D5-5B54-4F48-8C10-0A81788A91C7}" name="Category" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{DB00C74D-B328-4793-B628-EB0BE23D33E7}" name="Item" totalsRowFunction="count"/>
     <tableColumn id="4" xr3:uid="{0B7D84AA-C676-4203-B9FC-A71C7A990AF8}" name="Amount" totalsRowFunction="sum"/>
     <tableColumn id="5" xr3:uid="{9398C0CC-A231-44B1-A850-6246F2576D4A}" name="Major Expense ?">
@@ -6642,7 +6685,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E292182-348E-4DA0-8740-297B6F6A7C8B}" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E292182-348E-4DA0-8740-297B6F6A7C8B}" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:C6" xr:uid="{7E292182-348E-4DA0-8740-297B6F6A7C8B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{50E0E1EF-27FA-4779-B080-7AD292227C15}" name="Company"/>
@@ -6654,17 +6697,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1AD9ED95-18C7-417F-9134-7BD1DE1845DE}" name="Table4" displayName="Table4" ref="A1:E13" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1AD9ED95-18C7-417F-9134-7BD1DE1845DE}" name="Table4" displayName="Table4" ref="A1:E13" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A1:E13" xr:uid="{1AD9ED95-18C7-417F-9134-7BD1DE1845DE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
     <sortCondition ref="A1:A13"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E3D79CBA-E424-476E-AD6D-8C38622F6025}" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B849CC15-9321-4C09-B207-4D27D79C8A1F}" name="Category" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{7466C596-F506-434E-AA69-789CBCE2A5D2}" name="Item" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{89AE061A-8D1E-4581-8BEC-83604147F824}" name="Amount" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{910E468A-9413-4E5E-A98D-24B9B69575DA}" name="Major Expense ?" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E3D79CBA-E424-476E-AD6D-8C38622F6025}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{B849CC15-9321-4C09-B207-4D27D79C8A1F}" name="Category" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{7466C596-F506-434E-AA69-789CBCE2A5D2}" name="Item" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{89AE061A-8D1E-4581-8BEC-83604147F824}" name="Amount" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{910E468A-9413-4E5E-A98D-24B9B69575DA}" name="Major Expense ?" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6985,21 +7028,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="J1" s="7" t="s">
+      <c r="H1" s="13"/>
+      <c r="J1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="7"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -7285,7 +7328,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E13">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7622,7 +7665,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7657,13 +7700,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -7750,17 +7793,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="8"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -8014,7 +8057,7 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E13">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8042,17 +8085,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="J1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="8"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -8303,7 +8346,7 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E13">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8316,7 +8359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40E2687-F93C-47E2-8D02-CBA8CC0C25FA}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -8332,19 +8375,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -8355,20 +8398,20 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+      <c r="A2" s="8">
         <v>45413</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>500</v>
       </c>
-      <c r="E2" s="11" t="str">
-        <f>IF(D2&gt;=100,"YES","NO")</f>
+      <c r="E2" s="9" t="str">
+        <f t="shared" ref="E2:E12" si="0">IF(D2&gt;=100,"YES","NO")</f>
         <v>YES</v>
       </c>
       <c r="G2" t="s">
@@ -8380,20 +8423,20 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="8">
         <v>45413</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>100</v>
       </c>
-      <c r="E3" s="11" t="str">
-        <f>IF(D3&gt;=100,"YES","NO")</f>
+      <c r="E3" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="G3" t="s">
@@ -8405,20 +8448,20 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="10">
         <v>45413</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="11">
         <v>50</v>
       </c>
-      <c r="E4" s="13" t="str">
-        <f>IF(D4&gt;=100,"YES","NO")</f>
+      <c r="E4" s="11" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="G4" t="s">
@@ -8430,56 +8473,56 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="8">
         <v>45413</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>20</v>
       </c>
-      <c r="E5" s="11" t="str">
-        <f>IF(D5&gt;=100,"YES","NO")</f>
+      <c r="E5" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <v>45413</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="11">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="str">
-        <f>IF(D6&gt;=100,"YES","NO")</f>
+      <c r="E6" s="11" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <v>45414</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="11">
         <v>200</v>
       </c>
-      <c r="E7" s="13" t="str">
-        <f>IF(D7&gt;=100,"YES","NO")</f>
+      <c r="E7" s="11" t="str">
+        <f t="shared" si="0"/>
         <v>YES</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -8490,20 +8533,20 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="8">
         <v>45414</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>30</v>
       </c>
-      <c r="E8" s="11" t="str">
-        <f>IF(D8&gt;=100,"YES","NO")</f>
+      <c r="E8" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="G8" s="1">
@@ -8515,20 +8558,20 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
+      <c r="A9" s="10">
         <v>45414</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="11">
         <v>30</v>
       </c>
-      <c r="E9" s="13" t="str">
-        <f>IF(D9&gt;=100,"YES","NO")</f>
+      <c r="E9" s="11" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="G9" s="1">
@@ -8540,20 +8583,20 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="8">
         <v>45414</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>30</v>
       </c>
-      <c r="E10" s="11" t="str">
-        <f>IF(D10&gt;=100,"YES","NO")</f>
+      <c r="E10" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
       <c r="G10" s="1">
@@ -8565,61 +8608,61 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="10">
         <v>45414</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="11">
         <v>20</v>
       </c>
-      <c r="E11" s="13" t="str">
-        <f>IF(D11&gt;=100,"YES","NO")</f>
+      <c r="E11" s="11" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="8">
         <v>45415</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>90</v>
       </c>
-      <c r="E12" s="11" t="str">
-        <f>IF(D12&gt;=100,"YES","NO")</f>
+      <c r="E12" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="10">
         <v>45415</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="11">
         <v>70</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="11" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E12">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8629,4 +8672,296 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D703D4-30D1-4C07-AF61-96F98DF270EC}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="16">
+        <v>45046</v>
+      </c>
+      <c r="C2" s="16">
+        <v>45077</v>
+      </c>
+      <c r="D2" s="16">
+        <v>45107</v>
+      </c>
+      <c r="E2" s="16">
+        <v>45138</v>
+      </c>
+      <c r="F2" s="16">
+        <v>45169</v>
+      </c>
+      <c r="G2" s="16">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="20">
+        <v>100</v>
+      </c>
+      <c r="C3" s="20">
+        <v>85</v>
+      </c>
+      <c r="D3" s="20">
+        <v>87</v>
+      </c>
+      <c r="E3" s="20">
+        <v>73</v>
+      </c>
+      <c r="F3" s="20">
+        <v>68</v>
+      </c>
+      <c r="G3" s="20">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="20">
+        <v>42</v>
+      </c>
+      <c r="C4" s="20">
+        <v>37</v>
+      </c>
+      <c r="D4" s="20">
+        <v>38</v>
+      </c>
+      <c r="E4" s="20">
+        <v>32</v>
+      </c>
+      <c r="F4" s="20">
+        <v>18</v>
+      </c>
+      <c r="G4" s="20">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="20">
+        <v>12</v>
+      </c>
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="20">
+        <v>4</v>
+      </c>
+      <c r="E5" s="20">
+        <v>5</v>
+      </c>
+      <c r="F5" s="20">
+        <v>8</v>
+      </c>
+      <c r="G5" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="20">
+        <v>17</v>
+      </c>
+      <c r="C6" s="20">
+        <v>15</v>
+      </c>
+      <c r="D6" s="20">
+        <v>7</v>
+      </c>
+      <c r="E6" s="20">
+        <v>12</v>
+      </c>
+      <c r="F6" s="20">
+        <v>10</v>
+      </c>
+      <c r="G6" s="20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="20">
+        <v>29</v>
+      </c>
+      <c r="C7" s="20">
+        <v>32</v>
+      </c>
+      <c r="D7" s="20">
+        <v>38</v>
+      </c>
+      <c r="E7" s="20">
+        <v>24</v>
+      </c>
+      <c r="F7" s="20">
+        <v>32</v>
+      </c>
+      <c r="G7" s="20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="17">
+        <f>B7/B3</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C8" s="17">
+        <f t="shared" ref="C8:G8" si="0">C7/C3</f>
+        <v>0.37647058823529411</v>
+      </c>
+      <c r="D8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.43678160919540232</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.32876712328767121</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.29411764705882354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F35F8-A10B-4958-BDA3-ABA0081FB70C}">
+  <dimension ref="A3:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="22">
+        <v>100000</v>
+      </c>
+      <c r="C4" s="22">
+        <v>50000</v>
+      </c>
+      <c r="D4" s="22">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="22">
+        <v>150000</v>
+      </c>
+      <c r="C5" s="22">
+        <v>40000</v>
+      </c>
+      <c r="D5" s="22">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="22">
+        <v>87000</v>
+      </c>
+      <c r="C6" s="22">
+        <v>23000</v>
+      </c>
+      <c r="D6" s="22">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="22">
+        <v>125000</v>
+      </c>
+      <c r="C7" s="22">
+        <v>45000</v>
+      </c>
+      <c r="D7" s="22">
+        <v>170000</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="wDEeoRYVfJVhuwBQOh3WM/YjZltCzBjdKB81Zc3jxfQjcNFBUawdJwyvMpQIFNwcE/Xxmx4EMem/ZFLHEmhBzg==" saltValue="uMMNSuhaDqsu74yiq8sfUQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>